<commit_message>
Deploy full site refresh: improved navbar, mobile menu, styles, images
</commit_message>
<xml_diff>
--- a/blog/data for charts.xlsx
+++ b/blog/data for charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Luis\Business folder\tepuy_site\blog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFD84D1-A032-4870-AA45-A374895CF5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29AFFE2-EFDC-4F20-8127-C0E69DADC892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B159E2E-8423-4A54-869A-CB7D220BCCE4}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>